<commit_message>
changes since review with roxanne
</commit_message>
<xml_diff>
--- a/ReferenceFiles/TaskLists/gtProductAssembly010819.xlsx
+++ b/ReferenceFiles/TaskLists/gtProductAssembly010819.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10860" yWindow="300" windowWidth="17520" windowHeight="15520"/>
+    <workbookView xWindow="8620" yWindow="0" windowWidth="17520" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="8" r:id="rId1"/>
@@ -1561,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4538,7 +4538,7 @@
   <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6140,7 +6140,7 @@
   <dimension ref="A1:A68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6506,8 +6506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P89"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>